<commit_message>
Edit file: add attribute beschermlaag
</commit_message>
<xml_diff>
--- a/demo_bim4infra/basisimport.xlsx
+++ b/demo_bim4infra/basisimport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nordendeu-my.sharepoint.com/personal/dries_nordend_eu/Documents/projects/AWV/python_repositories/OTLMOW-PostenMapping/demo_bim4infra/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{C5E00183-BA74-4308-A84F-7F44E4EAF5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E744E963-1645-4B3F-BA5C-740F697D24AE}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{C5E00183-BA74-4308-A84F-7F44E4EAF5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FCA63CB-0D0C-4245-91CC-6D354791A3E4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>typeURI</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>beschermlaag</t>
+  </si>
+  <si>
+    <t>masthoogte</t>
   </si>
 </sst>
 </file>
@@ -474,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="I2" sqref="I2:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,9 +488,13 @@
     <col min="1" max="1" width="57.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,8 +522,11 @@
       <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -545,7 +555,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -571,7 +581,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -597,7 +607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -623,7 +633,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>

</xml_diff>